<commit_message>
Added QuestionBlock and Question Many to Many Relationship
</commit_message>
<xml_diff>
--- a/lms-service/src/test/resources/Java_question_1.xlsx
+++ b/lms-service/src/test/resources/Java_question_1.xlsx
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
-  <si>
-    <t>QuestionID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="68">
   <si>
     <t>Text</t>
   </si>
@@ -228,6 +225,12 @@
   </si>
   <si>
     <t>00000</t>
+  </si>
+  <si>
+    <t>QuestionBlock</t>
+  </si>
+  <si>
+    <t>Core Java</t>
   </si>
 </sst>
 </file>
@@ -273,10 +276,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,345 +561,336 @@
   <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <f>ROW()</f>
-        <v>2</v>
+      <c r="A2" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" t="s">
-        <v>14</v>
-      </c>
       <c r="O2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <f>ROW()</f>
-        <v>3</v>
+      <c r="A3" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
         <v>23</v>
       </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
       <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="O3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <f>ROW()</f>
-        <v>4</v>
+      <c r="A4" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" t="s">
         <v>27</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>28</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>29</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>30</v>
-      </c>
-      <c r="O4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <f>ROW()</f>
-        <v>5</v>
+      <c r="A5" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="O5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <f>ROW()</f>
-        <v>6</v>
+      <c r="A6" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <f>ROW()</f>
-        <v>7</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>44</v>
+      <c r="A7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="M7" s="1" t="s">
+      <c r="O7" t="s">
         <v>47</v>
-      </c>
-      <c r="O7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <f>ROW()</f>
-        <v>8</v>
+      <c r="A8" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="O8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <f>ROW()</f>
+      <c r="A9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L9" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="M9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <f>ROW()</f>
-        <v>10</v>
+      <c r="A10" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Assessment column changes from excel sheet.
</commit_message>
<xml_diff>
--- a/lms-service/src/test/resources/Java_question_1.xlsx
+++ b/lms-service/src/test/resources/Java_question_1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="71">
   <si>
     <t>Text</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>Java Thread</t>
+  </si>
+  <si>
+    <t>Basic Java</t>
+  </si>
+  <si>
+    <t>Assessment</t>
   </si>
 </sst>
 </file>
@@ -561,614 +567,672 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A19" sqref="A3:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>13</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
         <v>22</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>27</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>28</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>29</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>0</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1" t="s">
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
         <v>15</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>10</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>11</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>12</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>13</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
         <v>22</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>23</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>11</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>27</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>28</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>29</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="I16" s="1" t="s">
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K16" s="1">
         <v>0</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D17" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="I17" s="1" t="s">
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="P17" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="M18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="P18" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="I19" s="1" t="s">
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="P19" s="1" t="s">
         <v>63</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Proper Selection of collection for domain objects.
</commit_message>
<xml_diff>
--- a/lms-service/src/test/resources/Java_question_1.xlsx
+++ b/lms-service/src/test/resources/Java_question_1.xlsx
@@ -12,8 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7635"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="71">
   <si>
     <t>Text</t>
   </si>
@@ -567,20 +566,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A3:A19"/>
+      <selection sqref="A1:P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -630,7 +624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -665,7 +659,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -697,7 +691,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -729,7 +723,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -761,7 +755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -796,7 +790,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -831,7 +825,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -866,7 +860,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -898,7 +892,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -933,7 +927,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -968,7 +962,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -1000,7 +994,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -1032,7 +1026,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -1064,7 +1058,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1099,7 +1093,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -1134,7 +1128,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -1169,87 +1163,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Passing Score to Assessment, excel change STRING to text
</commit_message>
<xml_diff>
--- a/lms-service/src/test/resources/Java_question_1.xlsx
+++ b/lms-service/src/test/resources/Java_question_1.xlsx
@@ -53,9 +53,6 @@
     <t>Which of these standard collection classes implements a dynamic array?</t>
   </si>
   <si>
-    <t>STRING</t>
-  </si>
-  <si>
     <t>AbstractList</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>Assessment</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -569,17 +569,17 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P17"/>
+      <selection activeCell="E3" sqref="E3:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -603,22 +603,22 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>19</v>
-      </c>
-      <c r="O1" t="s">
-        <v>20</v>
       </c>
       <c r="P1" t="s">
         <v>7</v>
@@ -626,541 +626,541 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" t="s">
-        <v>13</v>
-      </c>
       <c r="P2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
       <c r="M3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="P3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" t="s">
         <v>26</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>27</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>28</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>29</v>
-      </c>
-      <c r="P4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="P5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="L6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="N7" s="1" t="s">
+      <c r="P7" t="s">
         <v>46</v>
-      </c>
-      <c r="P7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="P8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="N9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" t="s">
         <v>9</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>10</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>11</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>12</v>
       </c>
-      <c r="N11" t="s">
-        <v>13</v>
-      </c>
       <c r="P11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>22</v>
       </c>
-      <c r="L12" t="s">
-        <v>23</v>
-      </c>
       <c r="M12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="P12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" t="s">
         <v>26</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>27</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>28</v>
       </c>
-      <c r="N13" t="s">
+      <c r="P13" t="s">
         <v>29</v>
-      </c>
-      <c r="P13" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="P14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="L15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="K16" s="1">
         <v>0</v>
       </c>
       <c r="L16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="N16" s="1" t="s">
+      <c r="P16" t="s">
         <v>46</v>
-      </c>
-      <c r="P16" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="P17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Adding Passing Score to Assessment, excel change STRING to text"
This reverts commit e0fa71d59835beed6abeba6caf8473e4f8314dcb.
</commit_message>
<xml_diff>
--- a/lms-service/src/test/resources/Java_question_1.xlsx
+++ b/lms-service/src/test/resources/Java_question_1.xlsx
@@ -53,6 +53,9 @@
     <t>Which of these standard collection classes implements a dynamic array?</t>
   </si>
   <si>
+    <t>STRING</t>
+  </si>
+  <si>
     <t>AbstractList</t>
   </si>
   <si>
@@ -236,9 +239,6 @@
   </si>
   <si>
     <t>Assessment</t>
-  </si>
-  <si>
-    <t>text</t>
   </si>
 </sst>
 </file>
@@ -569,17 +569,17 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E17"/>
+      <selection sqref="A1:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -603,22 +603,22 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P1" t="s">
         <v>7</v>
@@ -626,541 +626,541 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="P6" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="P8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
       <c r="J15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="P15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H16">
         <v>1</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K16" s="1">
         <v>0</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
       <c r="J17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="P17" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding score, question block random and title flags, excel changes
</commit_message>
<xml_diff>
--- a/lms-service/src/test/resources/Java_question_1.xlsx
+++ b/lms-service/src/test/resources/Java_question_1.xlsx
@@ -53,9 +53,6 @@
     <t>Which of these standard collection classes implements a dynamic array?</t>
   </si>
   <si>
-    <t>STRING</t>
-  </si>
-  <si>
     <t>AbstractList</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>Assessment</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
@@ -569,17 +569,17 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P17"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -603,22 +603,22 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>19</v>
-      </c>
-      <c r="O1" t="s">
-        <v>20</v>
       </c>
       <c r="P1" t="s">
         <v>7</v>
@@ -626,541 +626,541 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
         <v>9</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>12</v>
       </c>
-      <c r="N2" t="s">
-        <v>13</v>
-      </c>
       <c r="P2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" t="s">
-        <v>23</v>
-      </c>
       <c r="M3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="P3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" t="s">
         <v>26</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>27</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>28</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>29</v>
-      </c>
-      <c r="P4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="P5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="L6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="N7" s="1" t="s">
+      <c r="P7" t="s">
         <v>46</v>
-      </c>
-      <c r="P7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="M8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="P8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="N9" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" t="s">
         <v>9</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>10</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>11</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>12</v>
       </c>
-      <c r="N11" t="s">
-        <v>13</v>
-      </c>
       <c r="P11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
         <v>21</v>
       </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>22</v>
       </c>
-      <c r="L12" t="s">
-        <v>23</v>
-      </c>
       <c r="M12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="P12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" t="s">
         <v>26</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>27</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>28</v>
       </c>
-      <c r="N13" t="s">
+      <c r="P13" t="s">
         <v>29</v>
-      </c>
-      <c r="P13" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="P14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="L15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="K16" s="1">
         <v>0</v>
       </c>
       <c r="L16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="N16" s="1" t="s">
+      <c r="P16" t="s">
         <v>46</v>
-      </c>
-      <c r="P16" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="M17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="P17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>